<commit_message>
Update Data Collection and add ESCO files
</commit_message>
<xml_diff>
--- a/Code/DataBase/database_size.xlsx
+++ b/Code/DataBase/database_size.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novasbe365-my.sharepoint.com/personal/32399_novasbe_pt/Documents/Work Project/Code/DataBase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novasbe365-my.sharepoint.com/personal/32399_novasbe_pt/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="514" documentId="11_F25DC773A252ABDACC1048E2595872AC5BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89A4154B-2599-438C-B3A4-0E7E31EF9B61}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BA51BC3-BD9B-4E5E-A872-13002F87CFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
   <si>
     <t>job_title</t>
   </si>
@@ -184,15 +184,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Size 60 Days</t>
-  </si>
-  <si>
-    <t>Size Historical Data</t>
-  </si>
-  <si>
-    <t>Last 60 Days</t>
-  </si>
-  <si>
     <t>Historical</t>
   </si>
   <si>
@@ -253,13 +244,16 @@
     <t>Size in 1 Week Scraping</t>
   </si>
   <si>
-    <t>Size with 60 days Scraped</t>
-  </si>
-  <si>
     <t>Yearly Cost assumming end of the Year Cost as per month</t>
   </si>
   <si>
     <t>Total Dataset Size</t>
+  </si>
+  <si>
+    <t>The number of records stored in one month is the number of records scraped/raw + the cleaned set, that is X*2</t>
+  </si>
+  <si>
+    <t>Amount Of Records Stored in 1 month</t>
   </si>
 </sst>
 </file>
@@ -500,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -539,7 +533,6 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -557,7 +550,186 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -709,149 +881,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1099,7 +1128,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$34</c:f>
+              <c:f>Sheet1!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1122,7 +1151,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$45</c:f>
+              <c:f>Sheet1!$B$27:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1164,42 +1193,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$35:$E$45</c:f>
+              <c:f>Sheet1!$C$27:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9.751345843359374</c:v>
+                  <c:v>6.5309765625000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.797071938593746</c:v>
+                  <c:v>15.54372421875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.364430124531246</c:v>
+                  <c:v>23.38089609375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.931788310468747</c:v>
+                  <c:v>31.218067968749999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.499146496406247</c:v>
+                  <c:v>39.055239843750002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58.066504682343748</c:v>
+                  <c:v>46.892411718750004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>67.633862868281255</c:v>
+                  <c:v>54.729583593750007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77.201221054218749</c:v>
+                  <c:v>62.56675546875001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>86.768579240156242</c:v>
+                  <c:v>70.403927343750013</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>96.335937426093736</c:v>
+                  <c:v>78.241099218750009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>105.90329561203123</c:v>
+                  <c:v>86.078271093750004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1215,7 +1244,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$34</c:f>
+              <c:f>Sheet1!$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1294,7 +1323,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$B$45</c:f>
+              <c:f>Sheet1!$B$27:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1336,42 +1365,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$35:$G$45</c:f>
+              <c:f>Sheet1!$E$27:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>_([$€-2]\ * #,##0_);_([$€-2]\ * \(#,##0\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.0126777820693746</c:v>
+                  <c:v>1.3479935625000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.086115648125749</c:v>
+                  <c:v>3.2082246787499997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0608183777032494</c:v>
+                  <c:v>4.8258169537499995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0355211072807489</c:v>
+                  <c:v>6.4434092287499993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.010223836858248</c:v>
+                  <c:v>8.0610015037499991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.98492656643575</c:v>
+                  <c:v>9.6785937787500007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.959629296013251</c:v>
+                  <c:v>11.296186053750002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.93433202559075</c:v>
+                  <c:v>12.913778328750002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.90903475516825</c:v>
+                  <c:v>14.531370603750002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.883737484745744</c:v>
+                  <c:v>16.148962878750002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.858440214323245</c:v>
+                  <c:v>17.766555153750001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2163,13 +2192,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1056245</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>65479</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>576471</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>50334</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2199,7 +2228,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61F520C6-C178-497E-9284-6B4CFE09A3FD}" name="Table1" displayName="Table1" ref="B2:G14" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61F520C6-C178-497E-9284-6B4CFE09A3FD}" name="Table1" displayName="Table1" ref="B2:G14" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="B2:G14" xr:uid="{61F520C6-C178-497E-9284-6B4CFE09A3FD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2209,49 +2238,43 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AE5AD334-7E3C-46AB-974F-AB2F26352F09}" name="Field Name" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{12219D86-2C7D-439A-9B3F-763FCCA10B11}" name="Data Type" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{E5BBEB3F-3785-4322-834E-0C869BEF4573}" name="Data Format" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{2388822C-1C8F-4C5A-9F7F-BF0BA6A98CD9}" name="Field Size" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{AE5AD334-7E3C-46AB-974F-AB2F26352F09}" name="Field Name" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{12219D86-2C7D-439A-9B3F-763FCCA10B11}" name="Data Type" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{E5BBEB3F-3785-4322-834E-0C869BEF4573}" name="Data Format" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{2388822C-1C8F-4C5A-9F7F-BF0BA6A98CD9}" name="Field Size" dataDxfId="20">
       <calculatedColumnFormula>J3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D0483127-526E-425B-8761-98F162311CDF}" name="Description" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{0938B1F0-3784-4ECD-893C-F4B139F7385C}" name="Example" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{D0483127-526E-425B-8761-98F162311CDF}" name="Description" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{0938B1F0-3784-4ECD-893C-F4B139F7385C}" name="Example" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{508BD03B-2E1C-4760-B7F9-FE8E7BE8EF2F}" name="Table3" displayName="Table3" ref="B34:G45" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B34:G45" xr:uid="{508BD03B-2E1C-4760-B7F9-FE8E7BE8EF2F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{508BD03B-2E1C-4760-B7F9-FE8E7BE8EF2F}" name="Table3" displayName="Table3" ref="B26:E38" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B26:E37" xr:uid="{508BD03B-2E1C-4760-B7F9-FE8E7BE8EF2F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FD8F6246-1E2F-40EA-880E-53AE4A51D0B0}" name="Year" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{1A9A91CC-8C0F-419C-A42B-4B5FDC5C7F11}" name="Size Historical Data" dataDxfId="12">
-      <calculatedColumnFormula>C34+$D$29*$C$48*$C$50</calculatedColumnFormula>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FD8F6246-1E2F-40EA-880E-53AE4A51D0B0}" name="Year" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1A9A91CC-8C0F-419C-A42B-4B5FDC5C7F11}" name="Total Dataset Size" dataDxfId="6" totalsRowDxfId="2">
+      <calculatedColumnFormula>C26+$D$21*$C$40*$C$42</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4BD8A9D7-E8A5-4C3F-9079-9FFB389CAE76}" name="Size 60 Days" dataDxfId="11">
-      <calculatedColumnFormula>$D$21*$C$49</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{A3CF573B-8D74-4A3A-86AA-156CD9343702}" name="Cost at end of the Year" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{75ECBAA3-9997-4AD0-ADC8-307224CCE8CE}" name="Yearly Cost assumming end of the Year Cost as per month" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(E27:E37)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DB33B473-16B9-4D20-A877-34EBC6BC7011}" name="Total Dataset Size" dataDxfId="10">
-      <calculatedColumnFormula>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{A3CF573B-8D74-4A3A-86AA-156CD9343702}" name="Cost at end of the Year" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{75ECBAA3-9997-4AD0-ADC8-307224CCE8CE}" name="Yearly Cost assumming end of the Year Cost as per month" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{17D3100D-942E-4725-A56F-262C0EE3E36F}" name="Table13" displayName="Table13" ref="D4:I16" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{17D3100D-942E-4725-A56F-262C0EE3E36F}" name="Table13" displayName="Table13" ref="D4:I16" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="D4:I16" xr:uid="{17D3100D-942E-4725-A56F-262C0EE3E36F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2261,12 +2284,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{57A85022-9360-461F-ADE3-327107BABE6C}" name="Field Name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{0A26C41C-A986-4B3B-90C3-E77F5059B27C}" name="Data Type" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B8E0B9CE-10E1-4CA5-9929-C2376A232213}" name="Data Format" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{53D206CD-48F9-4E7B-9F13-AC93017A2A1A}" name="Field Size" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{D958A00E-DAC6-4908-9DF0-AEEADDDC73FB}" name="Description" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{0BB665AC-ECEB-4CC5-A3FE-E3BD764B8523}" name="Example" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{57A85022-9360-461F-ADE3-327107BABE6C}" name="Field Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{0A26C41C-A986-4B3B-90C3-E77F5059B27C}" name="Data Type" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B8E0B9CE-10E1-4CA5-9929-C2376A232213}" name="Data Format" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{53D206CD-48F9-4E7B-9F13-AC93017A2A1A}" name="Field Size" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{D958A00E-DAC6-4908-9DF0-AEEADDDC73FB}" name="Description" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{0BB665AC-ECEB-4CC5-A3FE-E3BD764B8523}" name="Example" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2535,18 +2558,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="58.109375" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.109375" style="12" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="12"/>
@@ -2588,10 +2611,10 @@
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -2855,7 +2878,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7">
@@ -2990,29 +3013,25 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+        <v>49</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>45</v>
@@ -3023,32 +3042,27 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
       <c r="B19" s="16">
         <f>SUM($E$3:$E$14)</f>
         <v>1429</v>
       </c>
       <c r="C19" s="6">
-        <v>109869</v>
+        <f>45000*2</f>
+        <v>90000</v>
       </c>
       <c r="D19" s="6">
         <v>1024</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
       <c r="B20" s="18" t="s">
         <v>47</v>
       </c>
@@ -3056,684 +3070,446 @@
         <v>44</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
       <c r="B21" s="19">
         <v>0.2</v>
       </c>
       <c r="C21" s="6">
         <f>(1+B21)*$C$19</f>
-        <v>131842.79999999999</v>
+        <v>108000</v>
       </c>
       <c r="D21" s="20">
-        <f>(C21*$B$19/$D$19)*$C$49</f>
-        <v>183.98765742187499</v>
+        <f>(C21*$B$19/$D$19)*$C$41</f>
+        <v>150.71484375</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
       <c r="B22" s="19">
         <v>0</v>
       </c>
       <c r="C22" s="6">
         <f>(1+B22)*$C$19</f>
-        <v>109869</v>
+        <v>90000</v>
       </c>
       <c r="D22" s="20">
-        <f>(C22*$B$19/$D$19)*$C$49</f>
-        <v>153.32304785156251</v>
+        <f t="shared" ref="D22:D23" si="2">(C22*$B$19/$D$19)*$C$41</f>
+        <v>125.595703125</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
       <c r="B23" s="21">
         <v>-0.2</v>
       </c>
       <c r="C23" s="22">
         <f>(1+B23)*$C$19</f>
-        <v>87895.200000000012</v>
+        <v>72000</v>
       </c>
       <c r="D23" s="23">
-        <f>(C23*$B$19/$D$19)*$C$49</f>
-        <v>122.65843828125001</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>100.4765625</v>
+      </c>
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="16">
-        <f>SUM($E$3:$E$14)</f>
-        <v>1429</v>
-      </c>
-      <c r="C27" s="6">
-        <v>109869</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1024</v>
-      </c>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="26">
+        <f>$D$22*$C$40*$C$42</f>
+        <v>6.5309765625000002</v>
+      </c>
+      <c r="D27" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C27:C27)</f>
+        <v>0.112332796875</v>
+      </c>
+      <c r="E27" s="28">
+        <f t="shared" ref="E27:E37" si="3">D27*$C$43</f>
+        <v>1.3479935625000001</v>
+      </c>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C28" s="26">
+        <f>C27+$D$21*$C$40*$C$42*(1+$C$44)</f>
+        <v>15.54372421875</v>
+      </c>
+      <c r="D28" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C28:C28)</f>
+        <v>0.2673520565625</v>
+      </c>
+      <c r="E28" s="28">
+        <f t="shared" si="3"/>
+        <v>3.2082246787499997</v>
+      </c>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="C29" s="6">
-        <f>(1+B29)*$C$27</f>
-        <v>131842.79999999999</v>
-      </c>
-      <c r="D29" s="20">
-        <f>(C29*$B$19/$D$19)*$C$49</f>
-        <v>183.98765742187499</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="12">
+        <v>2024</v>
+      </c>
+      <c r="C29" s="26">
+        <f t="shared" ref="C29:C35" si="4">C28+$D$21*$C$40*$C$42</f>
+        <v>23.38089609375</v>
+      </c>
+      <c r="D29" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C29:C29)</f>
+        <v>0.4021514128125</v>
+      </c>
+      <c r="E29" s="28">
+        <f t="shared" si="3"/>
+        <v>4.8258169537499995</v>
+      </c>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="19">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6">
-        <f>(1+B30)*$C$27</f>
-        <v>109869</v>
-      </c>
-      <c r="D30" s="20">
-        <f>(C30*$B$19/$D$19)*$C$49</f>
-        <v>153.32304785156251</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C30" s="26">
+        <f t="shared" si="4"/>
+        <v>31.218067968749999</v>
+      </c>
+      <c r="D30" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C30:C30)</f>
+        <v>0.53695076906249994</v>
+      </c>
+      <c r="E30" s="28">
+        <f t="shared" si="3"/>
+        <v>6.4434092287499993</v>
+      </c>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="21">
-        <v>-0.2</v>
-      </c>
-      <c r="C31" s="22">
-        <f>(1+B31)*$C$27</f>
-        <v>87895.200000000012</v>
-      </c>
-      <c r="D31" s="23">
-        <f>(C31*$B$19/$D$19)*$C$49</f>
-        <v>122.65843828125001</v>
-      </c>
-      <c r="E31" s="26"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="12">
+        <v>2026</v>
+      </c>
+      <c r="C31" s="26">
+        <f t="shared" si="4"/>
+        <v>39.055239843750002</v>
+      </c>
+      <c r="D31" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C31:C31)</f>
+        <v>0.6717501253125</v>
+      </c>
+      <c r="E31" s="28">
+        <f t="shared" si="3"/>
+        <v>8.0610015037499991</v>
+      </c>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="12">
+        <v>2027</v>
+      </c>
+      <c r="C32" s="26">
+        <f t="shared" si="4"/>
+        <v>46.892411718750004</v>
+      </c>
+      <c r="D32" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C32:C32)</f>
+        <v>0.80654948156250006</v>
+      </c>
+      <c r="E32" s="28">
+        <f t="shared" si="3"/>
+        <v>9.6785937787500007</v>
+      </c>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="12">
+        <v>2028</v>
+      </c>
+      <c r="C33" s="26">
+        <f t="shared" si="4"/>
+        <v>54.729583593750007</v>
+      </c>
+      <c r="D33" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C33:C33)</f>
+        <v>0.94134883781250012</v>
+      </c>
+      <c r="E33" s="28">
+        <f t="shared" si="3"/>
+        <v>11.296186053750002</v>
+      </c>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="12"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="12">
+        <v>2029</v>
+      </c>
+      <c r="C34" s="26">
+        <f t="shared" si="4"/>
+        <v>62.56675546875001</v>
+      </c>
+      <c r="D34" s="27">
+        <f>MIN($C$47:$C$51)*SUM(C34:C34)</f>
+        <v>1.0761481940625002</v>
+      </c>
+      <c r="E34" s="28">
+        <f t="shared" si="3"/>
+        <v>12.913778328750002</v>
+      </c>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="12">
-        <v>2022</v>
-      </c>
-      <c r="C35" s="27">
-        <f>$D$29*$C$48*$C$50</f>
-        <v>9.5673581859374988</v>
+        <v>2030</v>
+      </c>
+      <c r="C35" s="26">
+        <f t="shared" si="4"/>
+        <v>70.403927343750013</v>
       </c>
       <c r="D35" s="27">
-        <f t="shared" ref="D35:D43" si="2">$D$21*$C$49</f>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E35" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>9.751345843359374</v>
-      </c>
-      <c r="F35" s="28">
-        <f t="shared" ref="F35:F45" si="3">MIN($C$55:$C$59)*SUM(C35:D35)</f>
-        <v>0.16772314850578124</v>
-      </c>
-      <c r="G35" s="29">
-        <f t="shared" ref="G35:G45" si="4">F35*$C$51</f>
-        <v>2.0126777820693746</v>
-      </c>
-      <c r="K35" s="12"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <f>MIN($C$47:$C$51)*SUM(C35:C35)</f>
+        <v>1.2109475503125002</v>
+      </c>
+      <c r="E35" s="28">
+        <f t="shared" si="3"/>
+        <v>14.531370603750002</v>
+      </c>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="12">
-        <v>2023</v>
-      </c>
-      <c r="C36" s="27">
-        <f>C35+$D$29*$C$48*$C$50*(1+$C$52)</f>
-        <v>19.613084281171872</v>
+        <v>2031</v>
+      </c>
+      <c r="C36" s="26">
+        <f t="shared" ref="C36:C37" si="5">C35+$D$21*$C$40*$C$42</f>
+        <v>78.241099218750009</v>
       </c>
       <c r="D36" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E36" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>19.797071938593746</v>
-      </c>
-      <c r="F36" s="28">
+        <f>MIN($C$47:$C$51)*SUM(C36:C36)</f>
+        <v>1.3457469065625001</v>
+      </c>
+      <c r="E36" s="28">
         <f t="shared" si="3"/>
-        <v>0.3405096373438124</v>
-      </c>
-      <c r="G36" s="29">
-        <f t="shared" si="4"/>
-        <v>4.086115648125749</v>
-      </c>
-      <c r="K36" s="12"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>16.148962878750002</v>
+      </c>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="12">
-        <v>2024</v>
-      </c>
-      <c r="C37" s="27">
-        <f t="shared" ref="C37:C43" si="5">C36+$D$29*$C$48*$C$50</f>
-        <v>29.180442467109373</v>
+        <v>2032</v>
+      </c>
+      <c r="C37" s="26">
+        <f t="shared" si="5"/>
+        <v>86.078271093750004</v>
       </c>
       <c r="D37" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E37" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>29.364430124531246</v>
-      </c>
-      <c r="F37" s="28">
+        <f>MIN($C$47:$C$51)*SUM(C37:C37)</f>
+        <v>1.4805462628125001</v>
+      </c>
+      <c r="E37" s="28">
         <f t="shared" si="3"/>
-        <v>0.50506819814193749</v>
-      </c>
-      <c r="G37" s="29">
-        <f t="shared" si="4"/>
-        <v>6.0608183777032494</v>
-      </c>
-      <c r="K37" s="12"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>17.766555153750001</v>
+      </c>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="12">
-        <v>2025</v>
-      </c>
-      <c r="C38" s="27">
-        <f t="shared" si="5"/>
-        <v>38.747800653046873</v>
-      </c>
-      <c r="D38" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E38" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>38.931788310468747</v>
-      </c>
-      <c r="F38" s="28">
-        <f t="shared" si="3"/>
-        <v>0.66962675894006241</v>
-      </c>
-      <c r="G38" s="29">
-        <f t="shared" si="4"/>
-        <v>8.0355211072807489</v>
-      </c>
-      <c r="K38" s="12"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="12">
-        <v>2026</v>
-      </c>
-      <c r="C39" s="27">
-        <f t="shared" si="5"/>
-        <v>48.315158838984374</v>
-      </c>
-      <c r="D39" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E39" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>48.499146496406247</v>
-      </c>
-      <c r="F39" s="28">
-        <f t="shared" si="3"/>
-        <v>0.83418531973818744</v>
-      </c>
-      <c r="G39" s="29">
-        <f t="shared" si="4"/>
-        <v>10.010223836858248</v>
-      </c>
-      <c r="K39" s="12"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="12">
-        <v>2027</v>
-      </c>
-      <c r="C40" s="27">
-        <f t="shared" si="5"/>
-        <v>57.882517024921874</v>
-      </c>
-      <c r="D40" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E40" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>58.066504682343748</v>
-      </c>
-      <c r="F40" s="28">
-        <f t="shared" si="3"/>
-        <v>0.99874388053631247</v>
-      </c>
-      <c r="G40" s="29">
-        <f t="shared" si="4"/>
-        <v>11.98492656643575</v>
-      </c>
-      <c r="K40" s="12"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="12">
-        <v>2028</v>
-      </c>
-      <c r="C41" s="27">
-        <f t="shared" si="5"/>
-        <v>67.449875210859375</v>
-      </c>
-      <c r="D41" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E41" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>67.633862868281255</v>
-      </c>
-      <c r="F41" s="28">
-        <f t="shared" si="3"/>
-        <v>1.1633024413344375</v>
-      </c>
-      <c r="G41" s="29">
-        <f t="shared" si="4"/>
-        <v>13.959629296013251</v>
-      </c>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="12">
-        <v>2029</v>
-      </c>
-      <c r="C42" s="27">
-        <f t="shared" si="5"/>
-        <v>77.017233396796868</v>
-      </c>
-      <c r="D42" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E42" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>77.201221054218749</v>
-      </c>
-      <c r="F42" s="28">
-        <f t="shared" si="3"/>
-        <v>1.3278610021325625</v>
-      </c>
-      <c r="G42" s="29">
-        <f t="shared" si="4"/>
-        <v>15.93433202559075</v>
-      </c>
-      <c r="K42" s="12"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="12">
-        <v>2030</v>
-      </c>
-      <c r="C43" s="27">
-        <f t="shared" si="5"/>
-        <v>86.584591582734362</v>
-      </c>
-      <c r="D43" s="27">
-        <f t="shared" si="2"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E43" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>86.768579240156242</v>
-      </c>
-      <c r="F43" s="28">
-        <f t="shared" si="3"/>
-        <v>1.4924195629306873</v>
-      </c>
-      <c r="G43" s="29">
-        <f t="shared" si="4"/>
-        <v>17.90903475516825</v>
-      </c>
-      <c r="K43" s="12"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="12">
-        <v>2031</v>
-      </c>
-      <c r="C44" s="27">
-        <f t="shared" ref="C44:C45" si="6">C43+$D$29*$C$48*$C$50</f>
-        <v>96.151949768671855</v>
-      </c>
-      <c r="D44" s="27">
-        <f t="shared" ref="D44:D45" si="7">$D$21*$C$49</f>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E44" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>96.335937426093736</v>
-      </c>
-      <c r="F44" s="28">
-        <f t="shared" si="3"/>
-        <v>1.6569781237288121</v>
-      </c>
-      <c r="G44" s="29">
-        <f t="shared" si="4"/>
-        <v>19.883737484745744</v>
-      </c>
-      <c r="K44" s="12"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="12">
-        <v>2032</v>
-      </c>
-      <c r="C45" s="27">
-        <f t="shared" si="6"/>
-        <v>105.71930795460935</v>
-      </c>
-      <c r="D45" s="27">
-        <f t="shared" si="7"/>
-        <v>0.18398765742187498</v>
-      </c>
-      <c r="E45" s="27">
-        <f>SUM(Table3[[#This Row],[Size Historical Data]:[Size 60 Days]])</f>
-        <v>105.90329561203123</v>
-      </c>
-      <c r="F45" s="28">
-        <f t="shared" si="3"/>
-        <v>1.8215366845269372</v>
-      </c>
-      <c r="G45" s="29">
-        <f t="shared" si="4"/>
-        <v>21.858440214323245</v>
-      </c>
-      <c r="K45" s="12"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E47" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" s="28">
-        <f>SUM(G35:G45)</f>
-        <v>131.73545709431437</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B48" s="30" t="s">
+      <c r="C38" s="26"/>
+      <c r="D38" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="28">
+        <f>SUM(E27:E37)</f>
+        <v>106.221892725</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="30">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="32">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="32">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="34">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="31">
-        <v>52</v>
+      <c r="D46" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="12">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C47" s="12">
+        <f>B47*0.86</f>
+        <v>1.9779999999999999E-2</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="12">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="C48" s="12">
+        <f>B48*0.86</f>
+        <v>1.7887999999999998E-2</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="33">
-        <v>1E-3</v>
+      <c r="B49" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="C49" s="12">
+        <f>B49*0.86</f>
+        <v>1.72E-2</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="33">
-        <v>1E-3</v>
+      <c r="B50" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C50" s="12">
+        <f>B50*0.86</f>
+        <v>1.8919999999999999E-2</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="33">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="35">
-        <v>0.05</v>
-      </c>
+      <c r="B51" s="12">
+        <v>2.5499999999999998E-2</v>
+      </c>
+      <c r="C51" s="12">
+        <f>B51*0.86</f>
+        <v>2.1929999999999998E-2</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="27"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="27"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="12">
-        <v>2.3E-2</v>
-      </c>
-      <c r="C55" s="12">
-        <f>B55*0.86</f>
-        <v>1.9779999999999999E-2</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>58</v>
-      </c>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="27"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="12">
-        <v>2.0799999999999999E-2</v>
-      </c>
-      <c r="C56" s="12">
-        <f>B56*0.86</f>
-        <v>1.7887999999999998E-2</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>59</v>
-      </c>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="27"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="C57" s="12">
-        <f>B57*0.86</f>
-        <v>1.72E-2</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>60</v>
-      </c>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="27"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="12">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="C58" s="12">
-        <f>B58*0.86</f>
-        <v>1.8919999999999999E-2</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="12">
-        <v>2.5499999999999998E-2</v>
-      </c>
-      <c r="C59" s="12">
-        <f>B59*0.86</f>
-        <v>2.1929999999999998E-2</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="28"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="28"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="28"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="28"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="28"/>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="28"/>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="28"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3947,7 +3723,7 @@
         <v>30</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="4:9" ht="26.4" x14ac:dyDescent="0.3">
@@ -4017,4 +3793,280 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F80895B69CCDD14CA0F9702F8D05C19F" ma:contentTypeVersion="12" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="102a4863fa8dc3c1581419704c621693">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f893dd06-06a5-4d5c-921f-658a734064c2" xmlns:ns4="77d4af12-420f-4a91-923e-b0047be253cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90b7634a16000de2b4a2e8cebadbebd7" ns3:_="" ns4:_="">
+    <xsd:import namespace="f893dd06-06a5-4d5c-921f-658a734064c2"/>
+    <xsd:import namespace="77d4af12-420f-4a91-923e-b0047be253cb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f893dd06-06a5-4d5c-921f-658a734064c2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="14" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="77d4af12-420f-4a91-923e-b0047be253cb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Partilhado Com" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalhes de Partilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Hash de Sugestão de Partilha" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0322D207-B11E-427D-AF36-D9A618A9D007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f893dd06-06a5-4d5c-921f-658a734064c2"/>
+    <ds:schemaRef ds:uri="77d4af12-420f-4a91-923e-b0047be253cb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94C4FC47-94C1-46BE-A04C-120612CDF489}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E635931-34F4-483D-9F0D-550D740684C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f893dd06-06a5-4d5c-921f-658a734064c2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="77d4af12-420f-4a91-923e-b0047be253cb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>